<commit_message>
data up to 1st
</commit_message>
<xml_diff>
--- a/doctor-visitsState.xlsx
+++ b/doctor-visitsState.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
   <si>
     <t>Alaska</t>
   </si>
@@ -537,6 +537,18 @@
   <si>
     <t>28 05 2020</t>
   </si>
+  <si>
+    <t>29 05 2020</t>
+  </si>
+  <si>
+    <t>30 05 2020</t>
+  </si>
+  <si>
+    <t>31 05 2020</t>
+  </si>
+  <si>
+    <t>01 06 2020</t>
+  </si>
 </sst>
 </file>
 
@@ -867,7 +879,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE119"/>
+  <dimension ref="A1:BE123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -19222,6 +19234,26 @@
         <v>173</v>
       </c>
     </row>
+    <row r="120" spans="1:57">
+      <c r="A120" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="121" spans="1:57">
+      <c r="A121" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="122" spans="1:57">
+      <c r="A122" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="123" spans="1:57">
+      <c r="A123" t="s">
+        <v>177</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>